<commit_message>
Added WS 2 (Error)
</commit_message>
<xml_diff>
--- a/inference_engine/inference_engine/temp.xlsx
+++ b/inference_engine/inference_engine/temp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="0" windowWidth="21560" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="14500" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>some</t>
   </si>
@@ -152,6 +152,72 @@
   </si>
   <si>
     <t>TK</t>
+  </si>
+  <si>
+    <t>sub det</t>
+  </si>
+  <si>
+    <t>sub noun</t>
+  </si>
+  <si>
+    <t>relation</t>
+  </si>
+  <si>
+    <t>obj det</t>
+  </si>
+  <si>
+    <t>obj noun</t>
+  </si>
+  <si>
+    <t>space relat</t>
+  </si>
+  <si>
+    <t>space det</t>
+  </si>
+  <si>
+    <t>space obj</t>
+  </si>
+  <si>
+    <t>time relat</t>
+  </si>
+  <si>
+    <t>time det</t>
+  </si>
+  <si>
+    <t>time obj</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>moment</t>
+  </si>
+  <si>
+    <t>moves</t>
+  </si>
+  <si>
+    <t>through</t>
+  </si>
+  <si>
+    <t>TRG</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>sub changed</t>
+  </si>
+  <si>
+    <t>obj changed</t>
+  </si>
+  <si>
+    <t>space obj changed</t>
+  </si>
+  <si>
+    <t>time obj changed</t>
   </si>
 </sst>
 </file>
@@ -217,8 +283,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -232,13 +300,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -693,10 +763,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -704,7 +774,7 @@
     <col min="6" max="6" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -715,9 +785,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -726,7 +796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -734,23 +804,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -760,8 +842,14 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -771,8 +859,14 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -782,8 +876,14 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -793,8 +893,14 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -804,16 +910,28 @@
       <c r="C10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -823,21 +941,117 @@
       <c r="C12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -845,6 +1059,7 @@
     <sortCondition ref="B1:B5"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>